<commit_message>
mobility-data-standard: fix bug in the xlsx file
</commit_message>
<xml_diff>
--- a/mobility-data-standard/mobility-data-standard.xlsx
+++ b/mobility-data-standard/mobility-data-standard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabularies\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713A10E7-392B-48C7-9E30-9AB40539A9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B128A2F-1738-403A-B973-F893E9103E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2130" yWindow="1575" windowWidth="21600" windowHeight="12585" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,7 +738,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" ref="A20:A31" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B20)," ","-"),",",""))</f>
+        <f t="shared" ref="A20:A32" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B20)," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/mobility-data-standard/ocit-c</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -860,6 +860,10 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/mobility-data-standard/other</v>
+      </c>
       <c r="B32" s="7" t="s">
         <v>37</v>
       </c>
@@ -954,6 +958,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4ea66b1c-fa60-4493-a86c-b420df37761a" xsi:nil="true"/>
+    <Date_x002f_Heure xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <note xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100156B981FAAFB4349A28B03AB4EEECF9F" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1e7c9bb6974a57a0073a8d48fc3b6089">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ea66b1c-fa60-4493-a86c-b420df37761a" xmlns:ns3="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d5753863158ce54f5fdf0d8971fe3971" ns2:_="" ns3:_="">
     <xsd:import namespace="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
@@ -1216,29 +1242,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4ea66b1c-fa60-4493-a86c-b420df37761a" xsi:nil="true"/>
-    <Date_x002f_Heure xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <note xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0610B8D-6EB9-4C25-8CE0-612AE3B494D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
+    <ds:schemaRef ds:uri="322c47a9-7cf9-4f39-ba36-4bf679c08fb0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60AB3605-D74C-42B6-A2DD-9EBC41B913EF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1255,23 +1278,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0610B8D-6EB9-4C25-8CE0-612AE3B494D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
-    <ds:schemaRef ds:uri="322c47a9-7cf9-4f39-ba36-4bf679c08fb0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>